<commit_message>
edits to fastq_J.PLAGGENBERG_12.10.19.xlsx and s1CDNASample_J.PLAGGENBERG_08.22.20.xlsx
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_J.PLAGGENBERG_12.10.19.xlsx
+++ b/fastqFiles/fastq_J.PLAGGENBERG_12.10.19.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="57">
   <si>
     <t xml:space="preserve">libraryDate</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">fastqFileName</t>
   </si>
   <si>
+    <t xml:space="preserve">NOTES</t>
+  </si>
+  <si>
     <t xml:space="preserve">11.15.19</t>
   </si>
   <si>
@@ -167,6 +170,9 @@
   </si>
   <si>
     <t xml:space="preserve">Brent_JP_72_GTAC_32_SIC_Index2_09_AAACCTT_TGTGAGGT_S33_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excluded from full run for low QC and tape station results. There are fastq files, but these are artifacts</t>
   </si>
   <si>
     <t xml:space="preserve">Brent_JP_75_GTAC_35_SIC_Index2_09_CGCTACA_TGTGAGGT_S36_R1_001.fastq.gz</t>
@@ -300,10 +306,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="M:Q"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T35" activeCellId="0" sqref="T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -353,13 +359,16 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
+      <c r="T1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>41</v>
@@ -368,13 +377,13 @@
         <v>4063</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>18.8</v>
@@ -386,15 +395,15 @@
         <v>2725211</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>42</v>
@@ -403,13 +412,13 @@
         <v>4063</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>31.1</v>
@@ -421,15 +430,15 @@
         <v>2707569</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>43</v>
@@ -438,13 +447,13 @@
         <v>4063</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>30.2</v>
@@ -456,15 +465,15 @@
         <v>2639020</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>44</v>
@@ -473,13 +482,13 @@
         <v>4063</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>14.4</v>
@@ -491,15 +500,15 @@
         <v>3045089</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>45</v>
@@ -508,13 +517,13 @@
         <v>4063</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>46.5</v>
@@ -526,15 +535,15 @@
         <v>2901630</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>46</v>
@@ -543,13 +552,13 @@
         <v>4063</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>13.3</v>
@@ -561,15 +570,15 @@
         <v>2622270</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>47</v>
@@ -578,13 +587,13 @@
         <v>4063</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>17.7</v>
@@ -596,15 +605,15 @@
         <v>2691537</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>48</v>
@@ -613,13 +622,13 @@
         <v>4063</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>18</v>
@@ -631,15 +640,15 @@
         <v>2870908</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>49</v>
@@ -648,13 +657,13 @@
         <v>4063</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>8.71</v>
@@ -666,15 +675,15 @@
         <v>2727448</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>50</v>
@@ -683,13 +692,13 @@
         <v>4063</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>59.1</v>
@@ -701,15 +710,15 @@
         <v>2550765</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>51</v>
@@ -718,13 +727,13 @@
         <v>4063</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>41.2</v>
@@ -736,15 +745,15 @@
         <v>2762436</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>52</v>
@@ -753,13 +762,13 @@
         <v>4063</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>18.8</v>
@@ -771,15 +780,15 @@
         <v>2853194</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>53</v>
@@ -788,13 +797,13 @@
         <v>4063</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>48.2</v>
@@ -806,15 +815,15 @@
         <v>3384915</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>54</v>
@@ -823,13 +832,13 @@
         <v>4063</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>30.9</v>
@@ -841,15 +850,15 @@
         <v>2913223</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>55</v>
@@ -858,13 +867,13 @@
         <v>4063</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>26.2</v>
@@ -876,15 +885,15 @@
         <v>2629133</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>56</v>
@@ -893,13 +902,13 @@
         <v>4063</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>12.5</v>
@@ -911,15 +920,15 @@
         <v>2879090</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>57</v>
@@ -928,13 +937,13 @@
         <v>4063</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>70.1</v>
@@ -946,15 +955,15 @@
         <v>2468028</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>58</v>
@@ -963,13 +972,13 @@
         <v>4063</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>52.9</v>
@@ -981,15 +990,15 @@
         <v>2681873</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>59</v>
@@ -998,13 +1007,13 @@
         <v>4063</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>66.6</v>
@@ -1016,15 +1025,15 @@
         <v>2730975</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>60</v>
@@ -1033,13 +1042,13 @@
         <v>4063</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>134</v>
@@ -1051,15 +1060,15 @@
         <v>2735171</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>61</v>
@@ -1068,13 +1077,13 @@
         <v>4063</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>41.3</v>
@@ -1086,15 +1095,15 @@
         <v>2866545</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>62</v>
@@ -1103,13 +1112,13 @@
         <v>4063</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>32.3</v>
@@ -1121,15 +1130,15 @@
         <v>3140919</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>63</v>
@@ -1138,13 +1147,13 @@
         <v>4063</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>21.8</v>
@@ -1156,15 +1165,15 @@
         <v>2810671</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>64</v>
@@ -1173,13 +1182,13 @@
         <v>4063</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>20.6</v>
@@ -1191,15 +1200,15 @@
         <v>2699102</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>65</v>
@@ -1208,13 +1217,13 @@
         <v>4063</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>20.3</v>
@@ -1226,15 +1235,15 @@
         <v>2727608</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>66</v>
@@ -1243,13 +1252,13 @@
         <v>4063</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>12.6</v>
@@ -1261,15 +1270,15 @@
         <v>2900510</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>67</v>
@@ -1278,13 +1287,13 @@
         <v>4063</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>31.2</v>
@@ -1296,15 +1305,15 @@
         <v>2743322</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>68</v>
@@ -1313,13 +1322,13 @@
         <v>4063</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>5.22</v>
@@ -1331,15 +1340,15 @@
         <v>3097863</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>69</v>
@@ -1348,13 +1357,13 @@
         <v>4063</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>54.9</v>
@@ -1366,15 +1375,15 @@
         <v>2615297</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>70</v>
@@ -1383,13 +1392,13 @@
         <v>4063</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>15.5</v>
@@ -1401,15 +1410,15 @@
         <v>2537281</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>71</v>
@@ -1418,13 +1427,13 @@
         <v>4063</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>20</v>
@@ -1436,15 +1445,15 @@
         <v>2863006</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>72</v>
@@ -1453,13 +1462,13 @@
         <v>4063</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>11.7</v>
@@ -1471,15 +1480,15 @@
         <v>2687924</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>73</v>
@@ -1488,13 +1497,13 @@
         <v>4063</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>0.508</v>
@@ -1505,13 +1514,16 @@
       <c r="K34" s="0" t="n">
         <v>735</v>
       </c>
+      <c r="T34" s="0" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>74</v>
@@ -1520,13 +1532,13 @@
         <v>4063</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>1.34</v>
@@ -1537,13 +1549,16 @@
       <c r="K35" s="0" t="n">
         <v>433</v>
       </c>
+      <c r="T35" s="0" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>75</v>
@@ -1552,13 +1567,13 @@
         <v>4063</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>44.4</v>
@@ -1570,15 +1585,15 @@
         <v>2521904</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>76</v>
@@ -1587,13 +1602,13 @@
         <v>4063</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I37" s="0" t="n">
         <v>19.4</v>
@@ -1605,15 +1620,15 @@
         <v>2482093</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>77</v>
@@ -1622,13 +1637,13 @@
         <v>4063</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I38" s="0" t="n">
         <v>26.5</v>
@@ -1640,15 +1655,15 @@
         <v>2551298</v>
       </c>
       <c r="L38" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>78</v>
@@ -1657,13 +1672,13 @@
         <v>4063</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I39" s="0" t="n">
         <v>51.9</v>
@@ -1675,15 +1690,15 @@
         <v>2803016</v>
       </c>
       <c r="L39" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>79</v>
@@ -1692,13 +1707,13 @@
         <v>4063</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>2.73</v>
@@ -1710,15 +1725,15 @@
         <v>2605959</v>
       </c>
       <c r="L40" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>80</v>
@@ -1727,13 +1742,13 @@
         <v>4063</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I41" s="0" t="n">
         <v>24.7</v>
@@ -1745,7 +1760,7 @@
         <v>2541767</v>
       </c>
       <c r="L41" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>